<commit_message>
TP2B revisar QuickSort arroja exception stackOverFlow
</commit_message>
<xml_diff>
--- a/TP2B/Documentacion/AnalisisRendimiento.xlsx
+++ b/TP2B/Documentacion/AnalisisRendimiento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ORDENADOS" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
   <si>
     <t>DATOS DEL EQUIPO DE PRUEBAS</t>
   </si>
@@ -89,7 +89,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +138,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -251,6 +257,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -269,7 +276,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1161,11 +1168,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150810992"/>
-        <c:axId val="150811552"/>
+        <c:axId val="159729104"/>
+        <c:axId val="159729664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150810992"/>
+        <c:axId val="159729104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,12 +1201,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150811552"/>
+        <c:crossAx val="159729664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150811552"/>
+        <c:axId val="159729664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,7 +1241,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150810992"/>
+        <c:crossAx val="159729104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1994,7 +2001,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2133,11 +2140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="151035312"/>
-        <c:axId val="151035872"/>
+        <c:axId val="160209984"/>
+        <c:axId val="160210544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151035312"/>
+        <c:axId val="160209984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,12 +2173,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151035872"/>
+        <c:crossAx val="160210544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151035872"/>
+        <c:axId val="160210544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2206,7 +2213,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151035312"/>
+        <c:crossAx val="160209984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2965,10 +2972,10 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>312</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3101,11 +3108,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="151246896"/>
-        <c:axId val="151247456"/>
+        <c:axId val="160408368"/>
+        <c:axId val="160408928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151246896"/>
+        <c:axId val="160408368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,12 +3141,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151247456"/>
+        <c:crossAx val="160408928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151247456"/>
+        <c:axId val="160408928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3174,7 +3181,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151246896"/>
+        <c:crossAx val="160408368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3596,7 +3603,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,34 +3615,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3644,23 +3651,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="12"/>
+      <c r="A4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -4036,7 +4043,7 @@
       <c r="I17" s="1">
         <v>0</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="1">
@@ -4062,7 +4069,7 @@
       <c r="I18" s="1">
         <v>2</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="1">
@@ -4088,8 +4095,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4101,34 +4108,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -4137,23 +4144,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="12"/>
+      <c r="A4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -4503,8 +4510,8 @@
       <c r="I16" s="1">
         <v>0</v>
       </c>
-      <c r="J16" s="17" t="s">
-        <v>20</v>
+      <c r="J16" s="18">
+        <v>125</v>
       </c>
       <c r="K16" s="1">
         <v>2</v>
@@ -4529,7 +4536,7 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="1">
@@ -4555,7 +4562,7 @@
       <c r="I18" s="1">
         <v>2</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="1">
@@ -4581,8 +4588,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4594,34 +4601,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -4630,23 +4637,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="12"/>
+      <c r="A4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -5022,8 +5029,8 @@
       <c r="I17" s="1">
         <v>3</v>
       </c>
-      <c r="J17" s="17" t="s">
-        <v>20</v>
+      <c r="J17" s="18">
+        <v>312</v>
       </c>
       <c r="K17" s="1">
         <v>8</v>
@@ -5048,8 +5055,8 @@
       <c r="I18" s="1">
         <v>4</v>
       </c>
-      <c r="J18" s="17" t="s">
-        <v>20</v>
+      <c r="J18" s="18">
+        <v>482</v>
       </c>
       <c r="K18" s="1">
         <v>15</v>

</xml_diff>

<commit_message>
TP2B casos de prueba
</commit_message>
<xml_diff>
--- a/TP2B/Documentacion/AnalisisRendimiento.xlsx
+++ b/TP2B/Documentacion/AnalisisRendimiento.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="ORDENADOS" sheetId="1" r:id="rId1"/>
     <sheet name="ORDEN INVERSO" sheetId="9" r:id="rId2"/>
     <sheet name="ALEATORIO" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -227,11 +227,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -254,6 +255,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -272,11 +274,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -294,7 +297,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -401,6 +404,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8185</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -477,6 +522,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1395</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5744</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -553,6 +640,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -629,6 +758,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -705,6 +876,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -781,6 +994,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7316</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -857,6 +1112,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -870,11 +1167,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160168736"/>
-        <c:axId val="160169296"/>
+        <c:axId val="169024896"/>
+        <c:axId val="169055744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160168736"/>
+        <c:axId val="169024896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,12 +1200,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160169296"/>
+        <c:crossAx val="169055744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160169296"/>
+        <c:axId val="169055744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +1240,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160168736"/>
+        <c:crossAx val="169024896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -968,7 +1265,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1079,6 +1376,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5583</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1155,6 +1494,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1348</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5473</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1231,6 +1612,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1307,6 +1730,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1383,6 +1848,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1459,6 +1966,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1535,6 +2084,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1548,11 +2139,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160384848"/>
-        <c:axId val="160385408"/>
+        <c:axId val="169008512"/>
+        <c:axId val="169084416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160384848"/>
+        <c:axId val="169008512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,12 +2172,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160385408"/>
+        <c:crossAx val="169084416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160385408"/>
+        <c:axId val="169084416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +2212,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160384848"/>
+        <c:crossAx val="169008512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1646,7 +2237,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1753,6 +2344,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12806</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53624</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1829,6 +2462,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11036</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1905,6 +2580,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1981,6 +2698,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2057,6 +2816,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2133,6 +2934,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9358</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2209,6 +3052,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2222,11 +3107,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160391568"/>
-        <c:axId val="160633024"/>
+        <c:axId val="169139584"/>
+        <c:axId val="169219584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160391568"/>
+        <c:axId val="169139584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,12 +3140,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160633024"/>
+        <c:crossAx val="169219584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160633024"/>
+        <c:axId val="169219584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +3180,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160391568"/>
+        <c:crossAx val="169139584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2469,7 +3354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2504,7 +3389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2716,8 +3601,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,34 +3614,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2765,23 +3650,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13"/>
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -2818,13 +3703,27 @@
       <c r="D5" s="10">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2836,13 +3735,27 @@
       <c r="D6" s="10">
         <v>100</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2854,151 +3767,319 @@
       <c r="D7" s="10">
         <v>1000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="10">
         <v>2000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>74</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="10">
         <v>3000</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="E9" s="1">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="10">
         <v>4000</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>17</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="10">
         <v>5000</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="E11" s="1">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="10">
         <v>6000</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>19</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="10">
         <v>7000</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="E13" s="1">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>37</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="10">
         <v>8000</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="E14" s="1">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1">
+        <v>33</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="10">
         <v>10000</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="E15" s="1">
+        <v>81</v>
+      </c>
+      <c r="F15" s="1">
+        <v>52</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>72</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="10">
         <v>20000</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="E16" s="1">
+        <v>328</v>
+      </c>
+      <c r="F16" s="1">
+        <v>215</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>282</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="10">
         <v>50000</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="1"/>
+      <c r="E17" s="1">
+        <v>2036</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1395</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1790</v>
+      </c>
+      <c r="K17" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="10">
         <v>100000</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="1"/>
+      <c r="E18" s="1">
+        <v>8185</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5744</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="11">
+        <v>7316</v>
+      </c>
+      <c r="K18" s="1">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3019,8 +4100,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,34 +4113,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3068,23 +4149,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13"/>
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -3121,13 +4202,27 @@
       <c r="D5" s="10">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3139,13 +4234,27 @@
       <c r="D6" s="10">
         <v>100</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -3157,151 +4266,319 @@
       <c r="D7" s="10">
         <v>1000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="E7" s="1">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>10</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="10">
         <v>2000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="E8" s="1">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>13</v>
+      </c>
+      <c r="K8" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="10">
         <v>3000</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="E9" s="1">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="10">
         <v>4000</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="E10" s="1">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="10">
         <v>5000</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="E11" s="1">
+        <v>64</v>
+      </c>
+      <c r="F11" s="1">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>17</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="10">
         <v>6000</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="E12" s="1">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>29</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="10">
         <v>7000</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="E13" s="1">
+        <v>112</v>
+      </c>
+      <c r="F13" s="1">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>35</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="10">
         <v>8000</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="E14" s="1">
+        <v>144</v>
+      </c>
+      <c r="F14" s="1">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="10">
         <v>10000</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="E15" s="1">
+        <v>225</v>
+      </c>
+      <c r="F15" s="1">
+        <v>51</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>74</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="10">
         <v>20000</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="1"/>
+      <c r="E16" s="1">
+        <v>896</v>
+      </c>
+      <c r="F16" s="1">
+        <v>216</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>288</v>
+      </c>
+      <c r="K16" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="10">
         <v>50000</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="1"/>
+      <c r="E17" s="1">
+        <v>5583</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1348</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1810</v>
+      </c>
+      <c r="K17" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="10">
         <v>100000</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="1"/>
+      <c r="E18" s="1">
+        <v>22702</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5473</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="11">
+        <v>7239</v>
+      </c>
+      <c r="K18" s="1">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3320,10 +4597,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3335,34 +4612,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3371,23 +4648,23 @@
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13"/>
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14"/>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -3424,13 +4701,27 @@
       <c r="D5" s="10">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3442,13 +4733,27 @@
       <c r="D6" s="10">
         <v>100</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -3460,151 +4765,320 @@
       <c r="D7" s="10">
         <v>1000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="E7" s="1">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="10">
         <v>2000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="E8" s="1">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="10">
         <v>3000</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="E9" s="1">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="10">
         <v>4000</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="E10" s="1">
+        <v>84</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="10">
         <v>5000</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="E11" s="1">
+        <v>115</v>
+      </c>
+      <c r="F11" s="1">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>13</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="10">
         <v>6000</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="E12" s="1">
+        <v>160</v>
+      </c>
+      <c r="F12" s="1">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="10">
         <v>7000</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="E13" s="1">
+        <v>219</v>
+      </c>
+      <c r="F13" s="1">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="10">
         <v>8000</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="E14" s="1">
+        <v>284</v>
+      </c>
+      <c r="F14" s="1">
+        <v>43</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>35</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="10">
         <v>10000</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="E15" s="1">
+        <v>449</v>
+      </c>
+      <c r="F15" s="1">
+        <v>68</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>60</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="10">
         <v>20000</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>1947</v>
+      </c>
+      <c r="F16" s="1">
+        <v>333</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>273</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="10">
         <v>50000</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>12806</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2550</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2132</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="10">
         <v>100000</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="1"/>
+      <c r="E18" s="1">
+        <v>53624</v>
+      </c>
+      <c r="F18" s="1">
+        <v>11036</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>5</v>
+      </c>
+      <c r="J18" s="11">
+        <v>9358</v>
+      </c>
+      <c r="K18" s="1">
+        <v>16</v>
+      </c>
+      <c r="L18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>